<commit_message>
Change to data sources
</commit_message>
<xml_diff>
--- a/DataSources/GLDW_DataSources.xlsx
+++ b/DataSources/GLDW_DataSources.xlsx
@@ -42,28 +42,13 @@
     <t>MJA Technology LLC</t>
   </si>
   <si>
-    <t>This is simulated data demonstrating how data from a series of buoys on Lake Erie could be graphed, analyzed and trigger alerts</t>
-  </si>
-  <si>
-    <t>TDSManual</t>
-  </si>
-  <si>
-    <t>TDSData</t>
-  </si>
-  <si>
     <t>Manual</t>
   </si>
   <si>
-    <t>This demonstrates how Total Dissolved Solids data that is manually entered can be validated prior to incorporating the data in the VDAB repository.</t>
-  </si>
-  <si>
     <t>Links</t>
   </si>
   <si>
     <t>&lt;a href='http://sources.gldw.org:40412/vdab'&gt;Container&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='http://sources.gldw.org:40402/vdab'&gt;Container&lt;/a&gt;&lt;hr&gt;&lt;a href='http://sources.gldw.org:40402/vdab/views/enterTDS'&gt;EntryForm&lt;/a&gt;</t>
   </si>
   <si>
     <t>High</t>
@@ -101,6 +86,21 @@
   <si>
     <t xml:space="preserve">&lt;a href='https://www.ndbc.noaa.gov/'&gt;National Data Buoy Center&lt;/a&gt;
 </t>
+  </si>
+  <si>
+    <t>This is simulated data demonstrating how data from a series of buoys on Lake Erie could be graphed, analyzed and trigger alerts. The NDBC data stream features actual buoy data.</t>
+  </si>
+  <si>
+    <t>SalinityData</t>
+  </si>
+  <si>
+    <t>SalinityProject</t>
+  </si>
+  <si>
+    <t>This demonstrates how specific conductivity data manually entered from a smartphone can be validated prior to incorporating the data in the GLDW  repository.</t>
+  </si>
+  <si>
+    <t>&lt;a href='http://sources.gldw.org:40402/vdab'&gt;Container&lt;/a&gt;&lt;hr&gt;&lt;a href='http://sources.gldw.org:40402/vdab/views/enterSalinity'&gt;EnterData&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,52 +481,52 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -538,30 +538,30 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refined the mapping for HAB Data
</commit_message>
<xml_diff>
--- a/DataSources/GLDW_DataSources.xlsx
+++ b/DataSources/GLDW_DataSources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Source</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>WaterMetrics</t>
-  </si>
-  <si>
-    <t>Simulated</t>
-  </si>
-  <si>
     <t>MJA Technology LLC</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>Links</t>
   </si>
   <si>
-    <t>&lt;a href='http://sources.gldw.org:40412/vdab'&gt;Container&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -67,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">This is data  read every 10 minutes from over 500 USGS monitoring stations. The water flow and water levels are read. GLDW Alerts are created for potential flooding conditions. </t>
-  </si>
-  <si>
-    <t>SimulatedBuoys</t>
   </si>
   <si>
     <t>NDBCBuoys</t>
@@ -88,9 +76,6 @@
 </t>
   </si>
   <si>
-    <t>This is simulated data demonstrating how data from a series of buoys on Lake Erie could be graphed, analyzed and trigger alerts. The NDBC data stream features actual buoy data.</t>
-  </si>
-  <si>
     <t>SalinityData</t>
   </si>
   <si>
@@ -101,6 +86,21 @@
   </si>
   <si>
     <t>&lt;a href='http://sources.gldw.org:40402/vdab'&gt;Container&lt;/a&gt;&lt;hr&gt;&lt;a href='http://sources.gldw.org:40402/vdab/views/enterSalinity'&gt;EnterData&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>WQDataStations</t>
+  </si>
+  <si>
+    <t>HABData</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Multiple Sources</t>
+  </si>
+  <si>
+    <t>This is Lake Erie data from stations that measure Chlorophyll and BlueGreen Algae levels.</t>
   </si>
 </sst>
 </file>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,87 +481,85 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>